<commit_message>
Oracle linked server and admin user in oracle
</commit_message>
<xml_diff>
--- a/Excel/Parametry_Systemu.xlsx
+++ b/Excel/Parametry_Systemu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jedrzej/MultiDB-Delivery-System/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MichalUrbaniak\Desktop\DeliveryDB\MultiDB-Delivery-System\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9521AE19-6B94-2840-AA1B-C519382336D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA2FE76-6EAB-4F2A-89D8-35935AE07A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="660" windowWidth="25380" windowHeight="27980" activeTab="1" xr2:uid="{EC61AF27-C861-2842-9A81-08BFB11E24D1}"/>
+    <workbookView xWindow="540" yWindow="1410" windowWidth="18060" windowHeight="11805" xr2:uid="{EC61AF27-C861-2842-9A81-08BFB11E24D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Parametry_Ogolne" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Parametr</t>
   </si>
@@ -61,15 +61,6 @@
   </si>
   <si>
     <t>MIN_WAGA_PACZKI</t>
-  </si>
-  <si>
-    <t>MAX_WAGA_PACZKI_A</t>
-  </si>
-  <si>
-    <t>MAX_WAGA_PACZKI_B</t>
-  </si>
-  <si>
-    <t>MAX_WAGA_PACZKI_C</t>
   </si>
   <si>
     <t>kg</t>
@@ -157,7 +148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -173,9 +164,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,7 +204,7 @@
         <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
@@ -319,7 +310,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -489,18 +480,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4840ECB8-3E28-134A-81C8-A894B2736BDC}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,7 +502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -519,10 +510,10 @@
         <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -533,7 +524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -541,10 +532,10 @@
         <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -552,10 +543,10 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -563,51 +554,18 @@
         <v>0.01</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
         <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -619,71 +577,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B05D315-68EB-504B-BFDD-361BE2C4E2FE}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="68.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="68.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>